<commit_message>
mmr + CW edits
</commit_message>
<xml_diff>
--- a/TABLE_PAPER.xlsx
+++ b/TABLE_PAPER.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nps01-my.sharepoint.com/personal/kurt_pasque_nps_edu/Documents/Desktop/NPS School Work/Thesis/TropicalNN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{81715F21-9F2A-4A01-89D4-72DC841C9B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F1DF4D6-CA8C-48C2-BC54-94AB5443FF86}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="8_{81715F21-9F2A-4A01-89D4-72DC841C9B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE4E36A1-1E61-4D4A-BA5E-C901D39F3214}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{04AA3A85-4489-49C7-8F2F-55A96556C0CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$F$810</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet3!$A$1:$F$810</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4808" uniqueCount="2580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4860" uniqueCount="2608">
   <si>
     <t>ReLU</t>
   </si>
@@ -7781,6 +7782,90 @@
   </si>
   <si>
     <t xml:space="preserve">Test Errors (% incorrect) </t>
+  </si>
+  <si>
+    <t>RELU</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>Total params: 23,719,498</t>
+  </si>
+  <si>
+    <t>Trainable params: 23,666,378</t>
+  </si>
+  <si>
+    <t>Non-trainable params: 53,120</t>
+  </si>
+  <si>
+    <t>Tropical</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Total params: 23,731,848</t>
+  </si>
+  <si>
+    <t>Trainable params: 23,678,728</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>+ FGSM AT</t>
+  </si>
+  <si>
+    <t>SVHN</t>
+  </si>
+  <si>
+    <t>Total params: 141,898</t>
+  </si>
+  <si>
+    <t>Trainable params: 141,898</t>
+  </si>
+  <si>
+    <t>Non-trainable params: 0</t>
+  </si>
+  <si>
+    <t>mnist 469</t>
+  </si>
+  <si>
+    <t>cifar 391</t>
+  </si>
+  <si>
+    <t>svhn 573</t>
+  </si>
+  <si>
+    <t>mnist 79</t>
+  </si>
+  <si>
+    <t>cifar 79</t>
+  </si>
+  <si>
+    <t>svhn 204</t>
+  </si>
+  <si>
+    <t>Test Accuracy Clean</t>
+  </si>
+  <si>
+    <t>Test Accuracy FGSM</t>
+  </si>
+  <si>
+    <t>Test Accuracy PGD Inf</t>
+  </si>
+  <si>
+    <t>Test Accuracy PGD 2</t>
+  </si>
+  <si>
+    <t>Test Accuracy CW</t>
+  </si>
+  <si>
+    <t>Test Accuracy SPSA</t>
+  </si>
+  <si>
+    <t>Batch size</t>
   </si>
 </sst>
 </file>
@@ -7788,7 +7873,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="181" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -8090,7 +8175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8121,16 +8206,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -8149,12 +8224,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8164,16 +8240,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8185,13 +8255,31 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8507,10 +8595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3172E9A4-AB67-485F-B0EF-209F270920E2}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="148" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="148" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8521,9 +8609,16 @@
     <col min="11" max="11" width="15.453125" customWidth="1"/>
     <col min="12" max="14" width="12.1796875" customWidth="1"/>
     <col min="15" max="15" width="12.453125" customWidth="1"/>
+    <col min="18" max="18" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="11" t="s">
@@ -8538,14 +8633,35 @@
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="33" t="s">
         <v>2577</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="R1" t="s">
+        <v>2601</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2602</v>
+      </c>
+      <c r="T1" t="s">
+        <v>2603</v>
+      </c>
+      <c r="U1" t="s">
+        <v>2604</v>
+      </c>
+      <c r="V1" t="s">
+        <v>2605</v>
+      </c>
+      <c r="W1" t="s">
+        <v>2606</v>
+      </c>
+      <c r="X1" t="s">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8570,16 +8686,37 @@
       <c r="H2" s="1" t="s">
         <v>2571</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="31" t="s">
         <v>2576</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="28" t="s">
         <v>2579</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
+      <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9516</v>
+      </c>
+      <c r="T2">
+        <v>0.87660000000000005</v>
+      </c>
+      <c r="U2">
+        <v>0.99139999999999995</v>
+      </c>
+      <c r="V2">
+        <v>6.6E-3</v>
+      </c>
+      <c r="W2">
+        <v>0.93410000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -8596,18 +8733,39 @@
       <c r="H3" s="1">
         <v>27.83</v>
       </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="37" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="21" t="s">
         <v>2575</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="21" t="s">
         <v>2574</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="Q3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0.99170000000000003</v>
+      </c>
+      <c r="S3">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="T3">
+        <v>0.89929999999999999</v>
+      </c>
+      <c r="U3">
+        <v>0.99019999999999997</v>
+      </c>
+      <c r="V3">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="W3">
+        <v>0.90580000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -8624,20 +8782,41 @@
       <c r="H4" s="1">
         <v>54.72</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="18">
         <v>17.760000000000005</v>
       </c>
-      <c r="M4" s="22">
+      <c r="M4" s="18">
         <v>88.92</v>
       </c>
-      <c r="N4" s="22">
+      <c r="N4" s="18">
         <v>72.17</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="Q4" t="s">
+        <v>2585</v>
+      </c>
+      <c r="R4">
+        <v>0.9929</v>
+      </c>
+      <c r="S4">
+        <v>0.97760000000000002</v>
+      </c>
+      <c r="T4">
+        <v>0.95889999999999997</v>
+      </c>
+      <c r="U4">
+        <v>0.99270000000000003</v>
+      </c>
+      <c r="V4">
+        <v>0.88580000000000003</v>
+      </c>
+      <c r="W4">
+        <v>0.97829999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -8654,20 +8833,20 @@
       <c r="H5" s="1">
         <v>39.25</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="15">
         <v>17.129999999999995</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="15">
         <v>90.08</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="15">
         <v>74.739999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -8684,20 +8863,20 @@
       <c r="H6" s="1">
         <v>55.1</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="15">
         <v>18.97</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="17">
         <v>77.010000000000005</v>
       </c>
-      <c r="N6" s="21">
+      <c r="N6" s="17">
         <v>60.75</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -8727,8 +8906,8 @@
         <v>-13.989999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>2572</v>
       </c>
       <c r="B8" s="1">
@@ -8757,7 +8936,7 @@
         <v>-11.420000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
@@ -8768,14 +8947,14 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="K9" s="24" t="s">
+      <c r="K9" s="34" t="s">
         <v>2578</v>
       </c>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
@@ -8786,16 +8965,16 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="26" t="s">
         <v>2576</v>
       </c>
-      <c r="L10" s="26" t="s">
+      <c r="L10" s="23" t="s">
         <v>2579</v>
       </c>
-      <c r="M10" s="27"/>
-      <c r="N10" s="28"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M10" s="24"/>
+      <c r="N10" s="25"/>
+    </row>
+    <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
         <v>31</v>
       </c>
@@ -8806,18 +8985,18 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="30" t="s">
+      <c r="K11" s="27"/>
+      <c r="L11" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="M11" s="30" t="s">
+      <c r="M11" s="20" t="s">
         <v>2575</v>
       </c>
-      <c r="N11" s="30" t="s">
+      <c r="N11" s="20" t="s">
         <v>2574</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>2573</v>
       </c>
@@ -8828,34 +9007,34 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="19">
         <v>27.689999999999998</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="19">
         <v>53.18</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="19">
         <v>45.28</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K13" s="20" t="s">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="K13" s="16" t="s">
         <v>2572</v>
       </c>
-      <c r="L13" s="20">
+      <c r="L13" s="16">
         <v>24.790000000000006</v>
       </c>
-      <c r="M13" s="20">
+      <c r="M13" s="16">
         <v>54.11</v>
       </c>
-      <c r="N13" s="20">
+      <c r="N13" s="16">
         <v>44.4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="11" t="s">
@@ -8870,20 +9049,20 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="20">
+      <c r="L14" s="16">
         <v>25.08</v>
       </c>
-      <c r="M14" s="20">
+      <c r="M14" s="16">
         <v>56.05</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="16">
         <v>44.9</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -8896,7 +9075,7 @@
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -8909,133 +9088,133 @@
         <v>2571</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="16">
-        <f>100-B3</f>
+      <c r="B16" s="12">
+        <f t="shared" ref="B16:B21" si="2">100-B3</f>
         <v>17.760000000000005</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16">
-        <f>100-G3</f>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12">
+        <f t="shared" ref="G16:H21" si="3">100-G3</f>
         <v>88.92</v>
       </c>
-      <c r="H16" s="16">
-        <f>100-H3</f>
+      <c r="H16" s="12">
+        <f t="shared" si="3"/>
         <v>72.17</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="18">
-        <f>100-B4</f>
+      <c r="B17" s="14">
+        <f t="shared" si="2"/>
         <v>27.689999999999998</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18">
-        <f>100-G4</f>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14">
+        <f t="shared" si="3"/>
         <v>53.18</v>
       </c>
-      <c r="H17" s="18">
-        <f>100-H4</f>
+      <c r="H17" s="14">
+        <f t="shared" si="3"/>
         <v>45.28</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="16">
-        <f>100-B5</f>
+      <c r="B18" s="12">
+        <f t="shared" si="2"/>
         <v>18.97</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17">
-        <f>100-G5</f>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13">
+        <f t="shared" si="3"/>
         <v>77.010000000000005</v>
       </c>
-      <c r="H18" s="17">
-        <f>100-H5</f>
+      <c r="H18" s="13">
+        <f t="shared" si="3"/>
         <v>60.75</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="18">
-        <f>100-B6</f>
+      <c r="B19" s="14">
+        <f t="shared" si="2"/>
         <v>25.08</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18">
-        <f>100-G6</f>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14">
+        <f t="shared" si="3"/>
         <v>56.05</v>
       </c>
-      <c r="H19" s="18">
-        <f>100-H6</f>
+      <c r="H19" s="14">
+        <f t="shared" si="3"/>
         <v>44.9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="16">
-        <f>100-B7</f>
+      <c r="B20" s="12">
+        <f t="shared" si="2"/>
         <v>17.129999999999995</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16">
-        <f>100-G7</f>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12">
+        <f t="shared" si="3"/>
         <v>90.08</v>
       </c>
-      <c r="H20" s="16">
-        <f>100-H7</f>
+      <c r="H20" s="12">
+        <f t="shared" si="3"/>
         <v>74.739999999999995</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="14" t="s">
         <v>2572</v>
       </c>
-      <c r="B21" s="18">
-        <f>100-B8</f>
+      <c r="B21" s="14">
+        <f t="shared" si="2"/>
         <v>24.790000000000006</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18">
-        <f>100-G8</f>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14">
+        <f t="shared" si="3"/>
         <v>54.11</v>
       </c>
-      <c r="H21" s="18">
-        <f>100-H8</f>
+      <c r="H21" s="14">
+        <f t="shared" si="3"/>
         <v>44.4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>21</v>
       </c>
@@ -9047,7 +9226,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>22</v>
       </c>
@@ -9059,7 +9238,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>31</v>
       </c>
@@ -9071,7 +9250,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>2573</v>
       </c>
@@ -9083,7 +9262,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F27">
         <v>640</v>
       </c>
@@ -9091,10 +9270,82 @@
         <v>23666378</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F28" s="38">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F28" s="22">
         <f>F27/G27</f>
         <v>2.7042583364467518E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I31" t="s">
+        <v>2595</v>
+      </c>
+      <c r="J31">
+        <v>469</v>
+      </c>
+      <c r="K31">
+        <f>J31*128</f>
+        <v>60032</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I32" t="s">
+        <v>2596</v>
+      </c>
+      <c r="J32">
+        <v>391</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ref="K32:K37" si="4">J32*128</f>
+        <v>50048</v>
+      </c>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I33" t="s">
+        <v>2597</v>
+      </c>
+      <c r="J33">
+        <v>573</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="4"/>
+        <v>73344</v>
+      </c>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I35" t="s">
+        <v>2598</v>
+      </c>
+      <c r="J35">
+        <v>79</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="4"/>
+        <v>10112</v>
+      </c>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I36" t="s">
+        <v>2599</v>
+      </c>
+      <c r="J36">
+        <v>79</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="4"/>
+        <v>10112</v>
+      </c>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I37" t="s">
+        <v>2600</v>
+      </c>
+      <c r="J37">
+        <v>204</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="4"/>
+        <v>26112</v>
       </c>
     </row>
   </sheetData>
@@ -9112,6 +9363,214 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC9AFF0-3D51-4CA3-B99D-9D87B79C3EF6}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>2589</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2580</v>
+      </c>
+      <c r="C2">
+        <v>2445.8247976303101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2581</v>
+      </c>
+      <c r="E2">
+        <v>6198.91155672073</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <f>C2/60</f>
+        <v>40.763746627171834</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2586</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2583</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2585</v>
+      </c>
+      <c r="C5">
+        <v>2394.3015499114899</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2581</v>
+      </c>
+      <c r="E5">
+        <v>6155.8655228614798</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2582</v>
+      </c>
+      <c r="M5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <f>C5/60</f>
+        <v>39.905025831858168</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2586</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2583</v>
+      </c>
+      <c r="M6">
+        <f>M5*300</f>
+        <v>18600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>2584</v>
+      </c>
+      <c r="M7">
+        <f>M6/60</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>2387.8790075778902</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2581</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2587</v>
+      </c>
+      <c r="M8">
+        <f>M7/60</f>
+        <v>5.166666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <f>C8/60</f>
+        <v>39.797983459631503</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>2591</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2580</v>
+      </c>
+      <c r="C11">
+        <v>540.25578212738003</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2581</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>2593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>2594</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>2591</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2585</v>
+      </c>
+      <c r="C14">
+        <v>457.36746358871397</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2581</v>
+      </c>
+      <c r="E14">
+        <v>915.06349611282303</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>2593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>2594</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>2591</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A44AEAB-ECCC-4F0A-AD29-671E9D93F54A}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -9130,16 +9589,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -9302,7 +9761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F418B82D-39F8-41BD-B29F-6385EE2194FE}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F810"/>

</xml_diff>